<commit_message>
reglage de bug + excel
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -26,7 +26,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="9">
     <fill>
       <patternFill/>
     </fill>
@@ -41,8 +41,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF0000"/>
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor rgb="FF00FFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFBF00"/>
+        <bgColor rgb="FFFFBF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -53,44 +59,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFBF00"/>
-        <bgColor rgb="FFFFBF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00FFFF"/>
-        <bgColor rgb="FF00FFFF"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF8080"/>
-        <bgColor rgb="FFFF8080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE3E3E3"/>
-        <bgColor rgb="FFE3E3E3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF69FFFF"/>
-        <bgColor rgb="FF69FFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -126,19 +102,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -513,9 +485,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.2" customWidth="1" min="1" max="1"/>
+    <col width="14.4" customWidth="1" min="1" max="1"/>
     <col width="25.2" customWidth="1" min="2" max="2"/>
-    <col width="27.6" customWidth="1" min="3" max="3"/>
+    <col width="25.2" customWidth="1" min="3" max="3"/>
     <col width="28.8" customWidth="1" min="4" max="4"/>
     <col width="28.8" customWidth="1" min="5" max="5"/>
     <col width="7.199999999999999" customWidth="1" min="6" max="6"/>
@@ -526,14 +498,14 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Semaine 5</t>
+          <t>Semaine 34</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>LUNDI</t>
+          <t>MERCREDI</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
@@ -574,31 +546,31 @@
           <t>VINGATARAMIN Pierre</t>
         </is>
       </c>
-      <c r="D4" s="3" t="inlineStr">
-        <is>
-          <t>HELFTER Franck</t>
-        </is>
-      </c>
-      <c r="G4" s="4" t="inlineStr">
-        <is>
-          <t>DA COSTA Nelson</t>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>BROGLIE Julien</t>
+        </is>
+      </c>
+      <c r="G4" s="3" t="inlineStr">
+        <is>
+          <t>FOECHTERLE Jean</t>
         </is>
       </c>
       <c r="H4" s="1" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>HORACEK Julien</t>
-        </is>
-      </c>
-      <c r="D5" s="3" t="inlineStr">
+      <c r="C5" s="4" t="inlineStr">
         <is>
           <t>SCHILLINGER  Jérémy</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>YEGEN Zulkifar</t>
         </is>
       </c>
     </row>
@@ -608,19 +580,19 @@
           <t>HUEBER Olivier</t>
         </is>
       </c>
-      <c r="D6" s="3" t="inlineStr">
-        <is>
-          <t>CAMARASA Sébastien</t>
-        </is>
-      </c>
-      <c r="G6" s="4" t="inlineStr">
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>WITZ Alain</t>
+        </is>
+      </c>
+      <c r="G6" s="3" t="inlineStr">
         <is>
           <t>GANTNER Stéphane</t>
         </is>
       </c>
       <c r="H6" s="1" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -631,26 +603,21 @@
           <t>B 2100</t>
         </is>
       </c>
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t>LUDAESCHER Olivier</t>
-        </is>
-      </c>
-      <c r="D8" s="3" t="inlineStr">
-        <is>
-          <t>DUCROT Déborah</t>
-        </is>
-      </c>
-      <c r="E8" s="5" t="inlineStr">
+      <c r="D8" s="4" t="inlineStr">
+        <is>
+          <t>HELFTER Franck</t>
+        </is>
+      </c>
+      <c r="E8" s="3" t="inlineStr">
+        <is>
+          <t>ABELLAN GRINAN Laurent</t>
+        </is>
+      </c>
+      <c r="G8" s="3" t="inlineStr">
         <is>
           <t>MORENO José</t>
         </is>
       </c>
-      <c r="G8" s="4" t="inlineStr">
-        <is>
-          <t>HAEFFELIN Dominique</t>
-        </is>
-      </c>
       <c r="H8" s="1" t="inlineStr">
         <is>
           <t>C</t>
@@ -658,46 +625,36 @@
       </c>
     </row>
     <row r="9">
-      <c r="C9" s="2" t="inlineStr">
-        <is>
-          <t>HAAG Patrick</t>
-        </is>
-      </c>
-      <c r="D9" s="3" t="inlineStr">
+      <c r="D9" s="4" t="inlineStr">
         <is>
           <t>ROUSSIN Frédéric</t>
         </is>
       </c>
-      <c r="E9" s="5" t="inlineStr">
-        <is>
-          <t>ABELLAN GRINAN Laurent</t>
+      <c r="E9" s="3" t="inlineStr">
+        <is>
+          <t>SCHAAL Eric</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="C10" s="2" t="inlineStr">
-        <is>
-          <t>SIMON Gael</t>
-        </is>
-      </c>
-      <c r="D10" s="5" t="inlineStr">
-        <is>
-          <t>YEGEN Zulkifar</t>
-        </is>
-      </c>
-      <c r="E10" s="5" t="inlineStr">
-        <is>
-          <t>SCHAAL Eric</t>
-        </is>
-      </c>
-      <c r="G10" s="4" t="inlineStr">
-        <is>
-          <t>MOSCOPOULOS Sébastien</t>
+      <c r="D10" s="4" t="inlineStr">
+        <is>
+          <t>LICHTLE Jean-Sébastien</t>
+        </is>
+      </c>
+      <c r="E10" s="4" t="inlineStr">
+        <is>
+          <t>Intérimaire</t>
+        </is>
+      </c>
+      <c r="G10" s="3" t="inlineStr">
+        <is>
+          <t>MULLER Gilbert</t>
         </is>
       </c>
       <c r="H10" s="1" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -708,48 +665,38 @@
           <t>B2000</t>
         </is>
       </c>
-      <c r="D12" s="3" t="inlineStr">
-        <is>
-          <t>BLATZ Jean-Marie</t>
-        </is>
-      </c>
-      <c r="E12" s="5" t="inlineStr">
+      <c r="C12" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">WOELFFLIN Gregory </t>
+        </is>
+      </c>
+      <c r="G12" s="3" t="inlineStr">
+        <is>
+          <t>SPIELMANN Patrice</t>
+        </is>
+      </c>
+      <c r="H12" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" s="3" t="inlineStr">
         <is>
           <t>RUBIO Alexandre</t>
         </is>
       </c>
-      <c r="G12" s="4" t="inlineStr">
-        <is>
-          <t>CORNOT David</t>
-        </is>
-      </c>
-      <c r="H12" s="1" t="inlineStr">
-        <is>
-          <t>nai</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="D13" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">WOELFFLIN Gregory </t>
-        </is>
-      </c>
-      <c r="E13" s="5" t="inlineStr">
-        <is>
-          <t>WITZ Alain</t>
-        </is>
-      </c>
     </row>
     <row r="14">
-      <c r="G14" s="4" t="inlineStr">
-        <is>
-          <t>DA SILVA David</t>
+      <c r="G14" s="3" t="inlineStr">
+        <is>
+          <t>TRAPANESE Antoine</t>
         </is>
       </c>
       <c r="H14" s="1" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -762,51 +709,66 @@
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>BUCHER Cyril</t>
-        </is>
-      </c>
-      <c r="D16" s="3" t="inlineStr">
-        <is>
-          <t>NESZCZADYN Franck</t>
-        </is>
-      </c>
-      <c r="G16" s="7" t="inlineStr">
-        <is>
-          <t>SCHREIBER Bertrand</t>
+          <t>GEIGER Frédéric</t>
+        </is>
+      </c>
+      <c r="D16" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="E16" s="3" t="inlineStr">
+        <is>
+          <t>FULLERINGER Gaétan</t>
+        </is>
+      </c>
+      <c r="G16" s="3" t="inlineStr">
+        <is>
+          <t>CORNOT David</t>
         </is>
       </c>
       <c r="H16" s="1" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="C17" s="2" t="inlineStr">
-        <is>
-          <t>GEIGER Frédéric</t>
-        </is>
-      </c>
-      <c r="D17" s="3" t="inlineStr">
-        <is>
-          <t>LICHTLE Jean-Sébastien</t>
+      <c r="C17" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="D17" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="E17" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>SIGWALT Thierry</t>
-        </is>
-      </c>
-      <c r="D18" s="5" t="inlineStr">
-        <is>
-          <t>FOECHTERLE Jean</t>
+          <t>HAAG Patrick</t>
+        </is>
+      </c>
+      <c r="D18" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="E18" s="4" t="inlineStr">
+        <is>
+          <t>LEROY Nicolas</t>
         </is>
       </c>
       <c r="G18" s="7" t="inlineStr">
         <is>
-          <t>EBRAN Vincent</t>
+          <t>DA SILVA David</t>
         </is>
       </c>
       <c r="H18" s="1" t="inlineStr">
@@ -822,42 +784,37 @@
           <t>DOMINO</t>
         </is>
       </c>
-      <c r="C20" s="2" t="inlineStr">
-        <is>
-          <t>BAUMANN Dylan</t>
-        </is>
-      </c>
-      <c r="D20" s="3" t="inlineStr">
-        <is>
-          <t>BERGER Virgil</t>
-        </is>
-      </c>
-      <c r="E20" s="5" t="inlineStr">
-        <is>
-          <t>SPIELMANN Patrice</t>
-        </is>
-      </c>
-      <c r="G20" s="7" t="inlineStr">
-        <is>
-          <t>LEDER Frédéric</t>
+      <c r="C20" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">KOESSEL Marc </t>
+        </is>
+      </c>
+      <c r="E20" s="3" t="inlineStr">
+        <is>
+          <t>DA COSTA Nelson</t>
+        </is>
+      </c>
+      <c r="G20" s="3" t="inlineStr">
+        <is>
+          <t>DANIEL Jean-Luc</t>
         </is>
       </c>
       <c r="H20" s="1" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="21"/>
     <row r="22">
-      <c r="G22" s="7" t="inlineStr">
-        <is>
-          <t>MOEGLING Vincent</t>
+      <c r="G22" s="3" t="inlineStr">
+        <is>
+          <t>FERDER Thomas</t>
         </is>
       </c>
       <c r="H22" s="1" t="inlineStr">
         <is>
-          <t>AP</t>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -868,29 +825,29 @@
           <t>PRESSE À BALLE</t>
         </is>
       </c>
-      <c r="C24" s="8" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
-        </is>
-      </c>
-      <c r="D24" s="3" t="inlineStr">
+      <c r="C24" s="2" t="inlineStr">
+        <is>
+          <t>SCHREIBER Bertrand</t>
+        </is>
+      </c>
+      <c r="D24" s="4" t="inlineStr">
         <is>
           <t>CORSET Christo</t>
         </is>
       </c>
-      <c r="E24" s="5" t="inlineStr">
-        <is>
-          <t>MULLER Gilbert</t>
+      <c r="E24" s="3" t="inlineStr">
+        <is>
+          <t>RITT Jean Jacques</t>
         </is>
       </c>
       <c r="G24" s="3" t="inlineStr">
         <is>
-          <t>LIZE Jonathan</t>
+          <t>FRICKERT Florian</t>
         </is>
       </c>
       <c r="H24" s="1" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -898,12 +855,12 @@
     <row r="26">
       <c r="G26" s="3" t="inlineStr">
         <is>
-          <t>GRIMONT Olivier</t>
+          <t>HOFFERT Patrick</t>
         </is>
       </c>
       <c r="H26" s="1" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -914,27 +871,27 @@
           <t>PLATEAUX</t>
         </is>
       </c>
-      <c r="G28" s="9" t="inlineStr">
-        <is>
-          <t>FIGUEIREDO José</t>
+      <c r="G28" s="3" t="inlineStr">
+        <is>
+          <t>LIER Romain</t>
         </is>
       </c>
       <c r="H28" s="1" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="29"/>
     <row r="30">
-      <c r="G30" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">KOESSEL Marc </t>
+      <c r="G30" s="3" t="inlineStr">
+        <is>
+          <t>MOZET Gaétan</t>
         </is>
       </c>
       <c r="H30" s="1" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -950,32 +907,27 @@
           <t>SUTTER Thierry</t>
         </is>
       </c>
-      <c r="D32" s="3" t="inlineStr">
-        <is>
-          <t>LEROY Nicolas</t>
-        </is>
-      </c>
-      <c r="E32" s="5" t="inlineStr">
+      <c r="E32" s="3" t="inlineStr">
         <is>
           <t>LOUIS Nicolas</t>
         </is>
       </c>
-      <c r="G32" s="9" t="inlineStr">
-        <is>
-          <t>MARTIN Hugues</t>
+      <c r="G32" s="3" t="inlineStr">
+        <is>
+          <t>RENCKER Michel</t>
         </is>
       </c>
       <c r="H32" s="1" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="33"/>
     <row r="34">
-      <c r="G34" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PINTO José </t>
+      <c r="G34" s="3" t="inlineStr">
+        <is>
+          <t>RUDLOFF Jérémy</t>
         </is>
       </c>
       <c r="H34" s="1" t="inlineStr">
@@ -993,40 +945,40 @@
       </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
-          <t>HAIL Fehrat</t>
-        </is>
-      </c>
-      <c r="D36" s="3" t="inlineStr">
-        <is>
-          <t>GUMUS Fatih</t>
-        </is>
-      </c>
-      <c r="E36" s="5" t="inlineStr">
-        <is>
-          <t>FRICKERT Florian</t>
-        </is>
-      </c>
-      <c r="G36" s="10" t="inlineStr">
-        <is>
-          <t>REIBEL Christophe</t>
+          <t>MOEGLING Vincent</t>
+        </is>
+      </c>
+      <c r="D36" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BOIREAU Stéphane </t>
+        </is>
+      </c>
+      <c r="E36" s="3" t="inlineStr">
+        <is>
+          <t>MOSCOPOULOS Sébastien</t>
+        </is>
+      </c>
+      <c r="G36" s="3" t="inlineStr">
+        <is>
+          <t>SCHENCK Emmanuel</t>
         </is>
       </c>
       <c r="H36" s="1" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="37"/>
     <row r="38">
-      <c r="G38" s="11" t="inlineStr">
-        <is>
-          <t>LUDAESCHER Pascal</t>
+      <c r="G38" s="2" t="inlineStr">
+        <is>
+          <t>BAUMANN Dylan</t>
         </is>
       </c>
       <c r="H38" s="1" t="inlineStr">
         <is>
-          <t>N*</t>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -1037,14 +989,35 @@
           <t>2T</t>
         </is>
       </c>
-      <c r="D40" s="12" t="inlineStr">
-        <is>
-          <t>VINCENT</t>
+      <c r="C40" s="8" t="inlineStr">
+        <is>
+          <t>Vincent WENDLING</t>
+        </is>
+      </c>
+      <c r="G40" s="2" t="inlineStr">
+        <is>
+          <t>BUCHER Cyril</t>
+        </is>
+      </c>
+      <c r="H40" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="41"/>
-    <row r="42"/>
+    <row r="42">
+      <c r="G42" s="7" t="inlineStr">
+        <is>
+          <t>CASPARD Gaël</t>
+        </is>
+      </c>
+      <c r="H42" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
     <row r="43"/>
     <row r="44">
       <c r="B44" s="1" t="inlineStr">
@@ -1057,14 +1030,19 @@
           <t>NETALA Frédéric</t>
         </is>
       </c>
-      <c r="D44" s="8" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>Personnel non affecté</t>
+      <c r="E44" s="3" t="inlineStr">
+        <is>
+          <t>GAVROY Gilles</t>
+        </is>
+      </c>
+      <c r="G44" s="2" t="inlineStr">
+        <is>
+          <t>HORACEK Julien</t>
+        </is>
+      </c>
+      <c r="H44" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -1074,26 +1052,31 @@
           <t>FRILLOT Jacky</t>
         </is>
       </c>
-      <c r="D45" s="8" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
+      <c r="E45" s="3" t="inlineStr">
+        <is>
+          <t>SPITZ Eric</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="C46" s="2" t="inlineStr">
         <is>
-          <t>HUGG Christian</t>
-        </is>
-      </c>
-      <c r="D46" s="8" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
-        </is>
-      </c>
-      <c r="G46" s="5" t="inlineStr">
-        <is>
-          <t>SPITZ Eric</t>
+          <t>AUDREN Olivier</t>
+        </is>
+      </c>
+      <c r="E46" s="4" t="inlineStr">
+        <is>
+          <t>SCANDELLA Christophe</t>
+        </is>
+      </c>
+      <c r="G46" s="2" t="inlineStr">
+        <is>
+          <t>LUDAESCHER Olivier</t>
+        </is>
+      </c>
+      <c r="H46" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -1109,14 +1092,19 @@
           <t>FUCHS Eric</t>
         </is>
       </c>
-      <c r="D48" s="3" t="inlineStr">
-        <is>
-          <t>FRITSCH Julien</t>
-        </is>
-      </c>
-      <c r="E48" s="5" t="inlineStr">
+      <c r="E48" s="3" t="inlineStr">
         <is>
           <t>VILLEMIN Franck</t>
+        </is>
+      </c>
+      <c r="G48" s="2" t="inlineStr">
+        <is>
+          <t>SIGWALT Thierry</t>
+        </is>
+      </c>
+      <c r="H48" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -1126,31 +1114,31 @@
           <t>FONTAINE Fabien</t>
         </is>
       </c>
-      <c r="D49" s="3" t="inlineStr">
-        <is>
-          <t>DA SILVA Axel</t>
-        </is>
-      </c>
-      <c r="E49" s="5" t="inlineStr">
-        <is>
-          <t>DANIEL Jean-Luc</t>
+      <c r="E49" s="3" t="inlineStr">
+        <is>
+          <t>FIGUEIREDO José</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="C50" s="5" t="inlineStr">
-        <is>
-          <t>MOZET Gaétan</t>
-        </is>
-      </c>
-      <c r="D50" s="3" t="inlineStr">
-        <is>
-          <t>SCANDELLA Christophe</t>
-        </is>
-      </c>
-      <c r="E50" s="5" t="inlineStr">
-        <is>
-          <t>GAVROY Gilles</t>
+      <c r="C50" s="2" t="inlineStr">
+        <is>
+          <t>LEDER Frédéric</t>
+        </is>
+      </c>
+      <c r="E50" s="3" t="inlineStr">
+        <is>
+          <t>GURLER Onur</t>
+        </is>
+      </c>
+      <c r="G50" s="2" t="inlineStr">
+        <is>
+          <t>SIMON Gael</t>
+        </is>
+      </c>
+      <c r="H50" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -1166,25 +1154,36 @@
           <t>SAHLI Halim</t>
         </is>
       </c>
-      <c r="D52" s="3" t="inlineStr">
-        <is>
-          <t>SCHWARZ Jean-Philippe</t>
+      <c r="G52" s="2" t="inlineStr">
+        <is>
+          <t>BELIANE Karim</t>
+        </is>
+      </c>
+      <c r="H52" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="C53" s="2" t="inlineStr">
         <is>
-          <t>AUDREN Olivier</t>
-        </is>
-      </c>
-      <c r="D53" s="5" t="inlineStr">
-        <is>
-          <t>RENCKER Michel</t>
-        </is>
-      </c>
-    </row>
-    <row r="54"/>
+          <t>EBRAN Vincent</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="G54" s="2" t="inlineStr">
+        <is>
+          <t>HIRSINGER Pascal</t>
+        </is>
+      </c>
+      <c r="H54" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
     <row r="55"/>
     <row r="56">
       <c r="B56" s="1" t="inlineStr">
@@ -1192,9 +1191,30 @@
           <t>SRE</t>
         </is>
       </c>
+      <c r="G56" s="2" t="inlineStr">
+        <is>
+          <t>HUGG Christian</t>
+        </is>
+      </c>
+      <c r="H56" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
     </row>
     <row r="57"/>
-    <row r="58"/>
+    <row r="58">
+      <c r="G58" s="2" t="inlineStr">
+        <is>
+          <t>RAKOTONDRAMANANA Nivo</t>
+        </is>
+      </c>
+      <c r="H58" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
     <row r="59"/>
     <row r="60">
       <c r="B60" s="1" t="inlineStr">
@@ -1202,14 +1222,40 @@
           <t>SMT</t>
         </is>
       </c>
-      <c r="C60" s="2" t="inlineStr">
-        <is>
-          <t>BELIANE Karim</t>
+      <c r="C60" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="D60" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="G60" s="2" t="inlineStr">
+        <is>
+          <t>RAMON Dominique</t>
+        </is>
+      </c>
+      <c r="H60" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="61"/>
-    <row r="62"/>
+    <row r="62">
+      <c r="G62" s="2" t="inlineStr">
+        <is>
+          <t>ROGLER Richard</t>
+        </is>
+      </c>
+      <c r="H62" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
     <row r="63"/>
     <row r="64">
       <c r="B64" s="1" t="inlineStr">
@@ -1217,14 +1263,35 @@
           <t>LBB1</t>
         </is>
       </c>
-      <c r="C64" s="6" t="inlineStr">
+      <c r="D64" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">ROTH Mathieu </t>
         </is>
       </c>
+      <c r="G64" s="4" t="inlineStr">
+        <is>
+          <t>BERGER Virgil</t>
+        </is>
+      </c>
+      <c r="H64" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
     </row>
     <row r="65"/>
-    <row r="66"/>
+    <row r="66">
+      <c r="G66" s="4" t="inlineStr">
+        <is>
+          <t>BLATZ Jean-Marie</t>
+        </is>
+      </c>
+      <c r="H66" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
     <row r="67"/>
     <row r="68">
       <c r="B68" s="1" t="inlineStr">
@@ -1234,12 +1301,33 @@
       </c>
       <c r="D68" s="6" t="inlineStr">
         <is>
-          <t xml:space="preserve">DJEBARA Philippe </t>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="G68" s="4" t="inlineStr">
+        <is>
+          <t>DUCROT Déborah</t>
+        </is>
+      </c>
+      <c r="H68" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="69"/>
-    <row r="70"/>
+    <row r="70">
+      <c r="G70" s="4" t="inlineStr">
+        <is>
+          <t>NESZCZADYN Franck</t>
+        </is>
+      </c>
+      <c r="H70" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
     <row r="71"/>
     <row r="72">
       <c r="B72" s="1" t="inlineStr">
@@ -1247,9 +1335,30 @@
           <t>MITR. BIMAC</t>
         </is>
       </c>
+      <c r="G72" s="4" t="inlineStr">
+        <is>
+          <t>BAUMANN Mike</t>
+        </is>
+      </c>
+      <c r="H72" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
     </row>
     <row r="73"/>
-    <row r="74"/>
+    <row r="74">
+      <c r="G74" s="4" t="inlineStr">
+        <is>
+          <t>FRITSCH Julien</t>
+        </is>
+      </c>
+      <c r="H74" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
     <row r="75"/>
     <row r="76">
       <c r="B76" s="1" t="inlineStr">
@@ -1259,22 +1368,43 @@
       </c>
       <c r="C76" s="2" t="inlineStr">
         <is>
-          <t>RAMON Dominique</t>
-        </is>
-      </c>
-      <c r="D76" s="3" t="inlineStr">
-        <is>
-          <t>BAUMANN Mike</t>
-        </is>
-      </c>
-      <c r="E76" s="5" t="inlineStr">
-        <is>
-          <t>HOFFERT Patrick</t>
+          <t>CASPAR Gaël</t>
+        </is>
+      </c>
+      <c r="D76" s="4" t="inlineStr">
+        <is>
+          <t>GRASSIN Axel</t>
+        </is>
+      </c>
+      <c r="E76" s="3" t="inlineStr">
+        <is>
+          <t>FRICKERT Rémy</t>
+        </is>
+      </c>
+      <c r="G76" s="4" t="inlineStr">
+        <is>
+          <t>GIDEMANN Olivier</t>
+        </is>
+      </c>
+      <c r="H76" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="77"/>
-    <row r="78"/>
+    <row r="78">
+      <c r="G78" s="4" t="inlineStr">
+        <is>
+          <t>GRIMONT Olivier</t>
+        </is>
+      </c>
+      <c r="H78" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
     <row r="79"/>
     <row r="80">
       <c r="B80" s="1" t="inlineStr">
@@ -1282,24 +1412,45 @@
           <t>PRÉPARATEUR</t>
         </is>
       </c>
-      <c r="C80" s="2" t="inlineStr">
-        <is>
-          <t>CASPAR Gaël</t>
-        </is>
-      </c>
-      <c r="D80" s="3" t="inlineStr">
-        <is>
-          <t>HERMANN Cédric</t>
-        </is>
-      </c>
-      <c r="E80" s="5" t="inlineStr">
-        <is>
-          <t>RITT Jean Jacques</t>
+      <c r="C80" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="D80" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="E80" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="G80" s="4" t="inlineStr">
+        <is>
+          <t>GUMUS Fatih</t>
+        </is>
+      </c>
+      <c r="H80" s="1" t="inlineStr">
+        <is>
+          <t>CF</t>
         </is>
       </c>
     </row>
     <row r="81"/>
-    <row r="82"/>
+    <row r="82">
+      <c r="G82" s="4" t="inlineStr">
+        <is>
+          <t>SCHWARZ Jean-Philippe</t>
+        </is>
+      </c>
+      <c r="H82" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
     <row r="83"/>
     <row r="84">
       <c r="B84" s="1" t="inlineStr">
@@ -1307,30 +1458,41 @@
           <t>M 1228</t>
         </is>
       </c>
-      <c r="D84" s="3" t="inlineStr">
-        <is>
-          <t>GRASSIN Axel</t>
-        </is>
-      </c>
-      <c r="E84" s="5" t="inlineStr">
-        <is>
-          <t>FRICKERT Rémy</t>
+      <c r="C84" s="2" t="inlineStr">
+        <is>
+          <t>HAIL Fehrat</t>
+        </is>
+      </c>
+      <c r="G84" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DJEBARA Philippe </t>
+        </is>
+      </c>
+      <c r="H84" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="85">
-      <c r="D85" s="8" t="inlineStr">
+      <c r="C85" s="6" t="inlineStr">
         <is>
           <t>Poste non affecté</t>
         </is>
       </c>
-      <c r="E85" s="5" t="inlineStr">
-        <is>
-          <t>GURLER Onur</t>
-        </is>
-      </c>
-    </row>
-    <row r="86"/>
+    </row>
+    <row r="86">
+      <c r="G86" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PINTO José </t>
+        </is>
+      </c>
+      <c r="H86" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
     <row r="87"/>
     <row r="88">
       <c r="B88" s="1" t="inlineStr">
@@ -1340,38 +1502,59 @@
       </c>
       <c r="C88" s="2" t="inlineStr">
         <is>
-          <t>HIRSINGER Pascal</t>
-        </is>
-      </c>
-      <c r="D88" s="3" t="inlineStr">
+          <t>HILDWEIN Steve</t>
+        </is>
+      </c>
+      <c r="D88" s="4" t="inlineStr">
         <is>
           <t>ANDRZEJEWSKI Nicolas</t>
         </is>
       </c>
-      <c r="E88" s="5" t="inlineStr">
-        <is>
-          <t>RUDLOFF Jérémy</t>
+      <c r="E88" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="G88" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PISKA Laurent </t>
+        </is>
+      </c>
+      <c r="H88" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="89">
-      <c r="C89" s="2" t="inlineStr">
-        <is>
-          <t>HILDWEIN Steve</t>
-        </is>
-      </c>
-      <c r="D89" s="3" t="inlineStr">
+      <c r="C89" s="4" t="inlineStr">
+        <is>
+          <t>HERMANN Cédric</t>
+        </is>
+      </c>
+      <c r="D89" s="4" t="inlineStr">
         <is>
           <t>BIELLMANN Cindy</t>
         </is>
       </c>
-      <c r="E89" s="5" t="inlineStr">
-        <is>
-          <t>SCHENCK Emmanuel</t>
-        </is>
-      </c>
-    </row>
-    <row r="90"/>
+      <c r="E89" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="G90" s="7" t="inlineStr">
+        <is>
+          <t>FRITSCH Patrick</t>
+        </is>
+      </c>
+      <c r="H90" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
     <row r="91"/>
     <row r="92">
       <c r="B92" s="1" t="inlineStr">
@@ -1381,17 +1564,22 @@
       </c>
       <c r="C92" s="2" t="inlineStr">
         <is>
-          <t>RAKOTONDRAMANANA Nivo</t>
-        </is>
-      </c>
-      <c r="D92" s="3" t="inlineStr">
+          <t>CAMACHO Michel</t>
+        </is>
+      </c>
+      <c r="E92" s="4" t="inlineStr">
         <is>
           <t>MASSINON Frédéric</t>
         </is>
       </c>
-      <c r="E92" s="5" t="inlineStr">
-        <is>
-          <t>FERDER Thomas</t>
+      <c r="G92" s="7" t="inlineStr">
+        <is>
+          <t>WENDLING Christophe</t>
+        </is>
+      </c>
+      <c r="H92" s="1" t="inlineStr">
+        <is>
+          <t>Nuit</t>
         </is>
       </c>
     </row>
@@ -1401,18 +1589,24 @@
           <t>ACKERMANN Rémy</t>
         </is>
       </c>
-      <c r="D93" s="3" t="inlineStr">
-        <is>
-          <t>PASQUIER Alexandre</t>
-        </is>
-      </c>
-      <c r="E93" s="5" t="inlineStr">
+      <c r="E93" s="3" t="inlineStr">
         <is>
           <t>ZWICKERT Xavier</t>
         </is>
       </c>
     </row>
-    <row r="94"/>
+    <row r="94">
+      <c r="G94" s="7" t="inlineStr">
+        <is>
+          <t>REIBEL Christophe</t>
+        </is>
+      </c>
+      <c r="H94" s="1" t="inlineStr">
+        <is>
+          <t>Mat</t>
+        </is>
+      </c>
+    </row>
     <row r="95"/>
     <row r="96">
       <c r="B96" s="1" t="inlineStr">
@@ -1420,40 +1614,41 @@
           <t>LMC</t>
         </is>
       </c>
-      <c r="C96" s="2" t="inlineStr">
-        <is>
-          <t>CAMACHO Michel</t>
-        </is>
-      </c>
-      <c r="D96" s="3" t="inlineStr">
-        <is>
-          <t>GIDEMANN Olivier</t>
-        </is>
-      </c>
-      <c r="E96" s="5" t="inlineStr">
-        <is>
-          <t>LIER Romain</t>
+      <c r="E96" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="G96" s="7" t="inlineStr">
+        <is>
+          <t>SIMLER Maurice</t>
+        </is>
+      </c>
+      <c r="H96" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="97">
-      <c r="C97" s="2" t="inlineStr">
-        <is>
-          <t>ROSSE Madeline</t>
-        </is>
-      </c>
-      <c r="D97" s="8" t="inlineStr">
+      <c r="E97" s="6" t="inlineStr">
         <is>
           <t>Poste non affecté</t>
         </is>
       </c>
-      <c r="E97" s="8" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
-        </is>
-      </c>
-    </row>
-    <row r="98"/>
+    </row>
+    <row r="98">
+      <c r="G98" s="4" t="inlineStr">
+        <is>
+          <t>LUDAESCHER Pascal</t>
+        </is>
+      </c>
+      <c r="H98" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
     <row r="99"/>
     <row r="100">
       <c r="B100" s="1" t="inlineStr">
@@ -1463,17 +1658,17 @@
       </c>
       <c r="C100" s="2" t="inlineStr">
         <is>
-          <t>ROGLER Richard</t>
-        </is>
-      </c>
-      <c r="D100" s="3" t="inlineStr">
+          <t>ROSSE Madeline</t>
+        </is>
+      </c>
+      <c r="D100" s="4" t="inlineStr">
         <is>
           <t>WEHRLEN Patrice</t>
         </is>
       </c>
-      <c r="E100" s="5" t="inlineStr">
-        <is>
-          <t>TRAPANESE Antoine</t>
+      <c r="E100" s="3" t="inlineStr">
+        <is>
+          <t>KIEFFER Victor</t>
         </is>
       </c>
     </row>
@@ -1491,19 +1686,25 @@
           <t>RIGOT Sébastien</t>
         </is>
       </c>
-      <c r="D104" s="3" t="inlineStr">
+      <c r="D104" s="4" t="inlineStr">
         <is>
           <t>VIAUD Cyril</t>
         </is>
       </c>
-      <c r="E104" s="8" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>Personnel non affecté</t>
         </is>
       </c>
     </row>
     <row r="105"/>
-    <row r="106"/>
+    <row r="106">
+      <c r="G106" s="4" t="inlineStr">
+        <is>
+          <t>DA SILVA Axel</t>
+        </is>
+      </c>
+    </row>
     <row r="107"/>
     <row r="108">
       <c r="B108" s="1" t="inlineStr">
@@ -1511,12 +1712,12 @@
           <t>HST</t>
         </is>
       </c>
-      <c r="C108" s="8" t="inlineStr">
+      <c r="C108" s="6" t="inlineStr">
         <is>
           <t>Poste non affecté</t>
         </is>
       </c>
-      <c r="D108" s="8" t="inlineStr">
+      <c r="D108" s="6" t="inlineStr">
         <is>
           <t>Poste non affecté</t>
         </is>

</xml_diff>